<commit_message>
Added feature what does not double row with remaining quantity to be delivered based on order status after call off (partial/ complete)
</commit_message>
<xml_diff>
--- a/deliveries_adding_OOP/data/calloff_template.xlsx
+++ b/deliveries_adding_OOP/data/calloff_template.xlsx
@@ -1251,7 +1251,7 @@
   <dimension ref="A1:L29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1305,20 +1305,20 @@
       <c r="A2" s="13">
         <v>44145</v>
       </c>
-      <c r="B2" s="19" t="s">
-        <v>12</v>
-      </c>
-      <c r="C2" s="19" t="s">
-        <v>14</v>
-      </c>
-      <c r="D2" s="20" t="s">
-        <v>15</v>
+      <c r="B2" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="22" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" s="23" t="s">
+        <v>17</v>
       </c>
       <c r="E2" s="21">
-        <v>1000</v>
+        <v>433</v>
       </c>
       <c r="F2" s="21">
-        <v>1000</v>
+        <v>433</v>
       </c>
       <c r="G2" s="13">
         <v>44150</v>
@@ -1327,10 +1327,10 @@
         <v>44150</v>
       </c>
       <c r="I2" s="21">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="J2" s="14" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="K2" s="3"/>
       <c r="L2" s="4"/>
@@ -1339,20 +1339,20 @@
       <c r="A3" s="13">
         <v>44145</v>
       </c>
-      <c r="B3" s="22" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" s="22" t="s">
-        <v>16</v>
-      </c>
-      <c r="D3" s="23" t="s">
-        <v>17</v>
+      <c r="B3" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" s="20" t="s">
+        <v>15</v>
       </c>
       <c r="E3" s="21">
-        <v>433</v>
+        <v>1000</v>
       </c>
       <c r="F3" s="21">
-        <v>433</v>
+        <v>1000</v>
       </c>
       <c r="G3" s="13">
         <v>44150</v>
@@ -1361,24 +1361,24 @@
         <v>44150</v>
       </c>
       <c r="I3" s="21">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="J3" s="14" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="K3" s="3"/>
       <c r="L3" s="4"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="11"/>
-      <c r="B4" s="15"/>
-      <c r="C4" s="15"/>
-      <c r="D4" s="16"/>
-      <c r="E4" s="12"/>
-      <c r="F4" s="12"/>
+      <c r="A4" s="13"/>
+      <c r="B4" s="22"/>
+      <c r="C4" s="22"/>
+      <c r="D4" s="23"/>
+      <c r="E4" s="21"/>
+      <c r="F4" s="21"/>
       <c r="G4" s="13"/>
       <c r="H4" s="13"/>
-      <c r="I4" s="12"/>
+      <c r="I4" s="21"/>
       <c r="J4" s="14"/>
       <c r="K4" s="3"/>
       <c r="L4" s="4"/>

</xml_diff>